<commit_message>
Repairs Module commit done
</commit_message>
<xml_diff>
--- a/InternalPortal/tcfile.xlsx
+++ b/InternalPortal/tcfile.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="174">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -47,7 +47,7 @@
     <t>Passed</t>
   </si>
   <si>
-    <t>2023-06-01</t>
+    <t>2023-06-06</t>
   </si>
   <si>
     <t>PERMNS_002_Verify_Branches_Permission_As_None</t>
@@ -197,6 +197,16 @@
     <t>PERMNS_040_Verify_Export_Permission_As_NoIn_Pricing</t>
   </si>
   <si>
+    <t>Import
+Add
+Filters</t>
+  </si>
+  <si>
+    <t>Top displayed text is Import
+Add
+Filters</t>
+  </si>
+  <si>
     <t>PERMNS_041_Verify_Import_Permission_As_Yes_In_Pricing</t>
   </si>
   <si>
@@ -231,6 +241,16 @@
     <t>PERMNS_044_Verify_Export_Permission_As_No_In_Discount Codes</t>
   </si>
   <si>
+    <t>Multi Edit
+Add
+Filters</t>
+  </si>
+  <si>
+    <t>Top displayed text is Multi Edit
+Add
+Filters</t>
+  </si>
+  <si>
     <t>PERMNS_044_Verify_Export_Permission_As_Yes_In_Non Standard Pricing</t>
   </si>
   <si>
@@ -243,6 +263,12 @@
   </si>
   <si>
     <t>PERMNS_045_Verify_Export_Permission_As_No_In_Non Standard Pricing</t>
+  </si>
+  <si>
+    <t>Pricing Rule Configurator</t>
+  </si>
+  <si>
+    <t>Top displayed text is Pricing Rule Configurator</t>
   </si>
   <si>
     <t>PERMNS_046_Verify_Pricing_Permission_As_View</t>
@@ -311,6 +337,130 @@
     <t>PERMNS_054_Verify_QuoteForParts_Permission_As_View</t>
   </si>
   <si>
+    <t>PERMNS_055_Verify_CreateSalesOrder_Permission_As_No_Quotes</t>
+  </si>
+  <si>
+    <t>PERMNS_056_Verify_CreateSalesOrder_Permission_As_Yes_Quotes</t>
+  </si>
+  <si>
+    <t>Create Sales Order</t>
+  </si>
+  <si>
+    <t>Top displayed text is Create Sales Order</t>
+  </si>
+  <si>
+    <t>PERMNS_057_Verify_QuoteClose_Permission_As_No_Quotes</t>
+  </si>
+  <si>
+    <t>Re Open</t>
+  </si>
+  <si>
+    <t>Top displayed text is Re Open</t>
+  </si>
+  <si>
+    <t>PERMNS_058_Verify_QuoteClose_Permission_As_Yes_Quotes</t>
+  </si>
+  <si>
+    <t>Re Open
+Close</t>
+  </si>
+  <si>
+    <t>Top displayed text is Re Open
+Close</t>
+  </si>
+  <si>
+    <t>PERMNS_059_Verify_Edit_IIDM_Cost_Permission_As_No_Quotes</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>Top displayed text is true</t>
+  </si>
+  <si>
+    <t>PERMNS_060_Verify_Edit_IIDM_Cost_Permission_As_Yes_Quotes</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>Top displayed text is null</t>
+  </si>
+  <si>
+    <t>PERMNS_061_Verify_ReOpen_Permission_As_No_Quotes</t>
+  </si>
+  <si>
+    <t>Close</t>
+  </si>
+  <si>
+    <t>Top displayed text is Close</t>
+  </si>
+  <si>
+    <t>PERMNS_062_Verify_ReOpen_Permission_As_Yes_Quotes</t>
+  </si>
+  <si>
+    <t>PERMNS_063_Verify_ReviseQuote_Permission_As_No_Quotes</t>
+  </si>
+  <si>
+    <t>Submit for Customer Approval</t>
+  </si>
+  <si>
+    <t>Top displayed text is Submit for Customer Approval</t>
+  </si>
+  <si>
+    <t>PERMNS_064_Verify_ReviseQuote_Permission_As_Yes_Quotes</t>
+  </si>
+  <si>
+    <t>Revise Quote
+Submit for Customer Approval</t>
+  </si>
+  <si>
+    <t>Top displayed text is Revise Quote
+Submit for Customer Approval</t>
+  </si>
+  <si>
+    <t>PERMNS_065_Verify_Send To Customer_Permission_As_No_Quotes</t>
+  </si>
+  <si>
+    <t>Revise Quote</t>
+  </si>
+  <si>
+    <t>Top displayed text is Revise Quote</t>
+  </si>
+  <si>
+    <t>PERMNS_066_Verify_Send To Customer_Permission_As_Yes_Quotes</t>
+  </si>
+  <si>
+    <t>PERMNS_067_Verify_Pay Terms_Permission_As_No_Quotes</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Top displayed text is 6</t>
+  </si>
+  <si>
+    <t>PERMNS_068_Verify_Pay Terms__Permission_As_Yes_Quotes</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>Top displayed text is 32</t>
+  </si>
+  <si>
+    <t>PERMNS_069_Verify_Quote Approval Limit__Permission_As_None_Quotes</t>
+  </si>
+  <si>
+    <t>PERMNS_070	_Verify_Quote Approval Limit__Permission_As_$50k and above_Quotes</t>
+  </si>
+  <si>
+    <t>Approve</t>
+  </si>
+  <si>
+    <t>Top displayed text is Approve</t>
+  </si>
+  <si>
     <t>PERMNS_071_Verify_Inventory_Permission_As_None</t>
   </si>
   <si>
@@ -389,9 +539,6 @@
   </si>
   <si>
     <t>PERMNS_085_Verify_Export_Permission_As_Yes_Organizations</t>
-  </si>
-  <si>
-    <t>PERMNS_086_Verify_Sync_Permission_As_Yes_Contacts</t>
   </si>
   <si>
     <t>Top displayed text is Save View
@@ -403,6 +550,19 @@
     <t>Save View
 Sync
 Export
+Filters</t>
+  </si>
+  <si>
+    <t>PERMNS_086_Verify_Sync_Permission_As_Yes_Contacts</t>
+  </si>
+  <si>
+    <t>Top displayed text is Save View
+Sync
+Filters</t>
+  </si>
+  <si>
+    <t>Save View
+Sync
 Filters</t>
   </si>
   <si>
@@ -494,7 +654,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
@@ -552,6 +712,22 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
@@ -565,7 +741,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
@@ -581,7 +757,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:F95"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -1392,10 +1568,10 @@
         <v>58</v>
       </c>
       <c r="B41" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C41" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D41" t="s">
         <v>9</v>
@@ -1409,7 +1585,7 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B42" t="s">
         <v>56</v>
@@ -1429,13 +1605,13 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B43" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C43" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D43" t="s">
         <v>9</v>
@@ -1449,13 +1625,13 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B44" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C44" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D44" t="s">
         <v>9</v>
@@ -1469,13 +1645,13 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B45" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C45" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D45" t="s">
         <v>9</v>
@@ -1489,13 +1665,13 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B46" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C46" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D46" t="s">
         <v>9</v>
@@ -1509,13 +1685,13 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B47" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="C47" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="D47" t="s">
         <v>9</v>
@@ -1529,13 +1705,13 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="B48" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C48" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="D48" t="s">
         <v>9</v>
@@ -1549,13 +1725,13 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="B49" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="C49" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="D49" t="s">
         <v>9</v>
@@ -1569,10 +1745,10 @@
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="B50" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C50" t="s">
         <v>8</v>
@@ -1589,13 +1765,13 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B51" t="s">
         <v>7</v>
       </c>
       <c r="C51" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="D51" t="s">
         <v>9</v>
@@ -1609,13 +1785,13 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B52" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="C52" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="D52" t="s">
         <v>9</v>
@@ -1629,13 +1805,13 @@
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B53" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C53" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="D53" t="s">
         <v>9</v>
@@ -1649,13 +1825,13 @@
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B54" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C54" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="D54" t="s">
         <v>9</v>
@@ -1669,13 +1845,13 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B55" t="s">
         <v>7</v>
       </c>
       <c r="C55" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="D55" t="s">
         <v>9</v>
@@ -1689,13 +1865,13 @@
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B56" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="C56" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="D56" t="s">
         <v>9</v>
@@ -1709,19 +1885,19 @@
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B57" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="C57" t="s">
-        <v>92</v>
+        <v>8</v>
       </c>
       <c r="D57" t="s">
         <v>9</v>
       </c>
-      <c r="E57" t="s">
-        <v>51</v>
+      <c r="E57" t="s" s="1">
+        <v>10</v>
       </c>
       <c r="F57" t="s">
         <v>11</v>
@@ -1729,13 +1905,13 @@
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="B58" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="C58" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="D58" t="s">
         <v>9</v>
@@ -1749,13 +1925,13 @@
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B59" t="s">
-        <v>7</v>
+        <v>102</v>
       </c>
       <c r="C59" t="s">
-        <v>8</v>
+        <v>103</v>
       </c>
       <c r="D59" t="s">
         <v>9</v>
@@ -1769,13 +1945,13 @@
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="B60" t="s">
-        <v>78</v>
+        <v>105</v>
       </c>
       <c r="C60" t="s">
-        <v>8</v>
+        <v>106</v>
       </c>
       <c r="D60" t="s">
         <v>9</v>
@@ -1789,13 +1965,13 @@
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="B61" t="s">
-        <v>7</v>
+        <v>108</v>
       </c>
       <c r="C61" t="s">
-        <v>80</v>
+        <v>109</v>
       </c>
       <c r="D61" t="s">
         <v>9</v>
@@ -1809,13 +1985,13 @@
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="B62" t="s">
-        <v>7</v>
+        <v>111</v>
       </c>
       <c r="C62" t="s">
-        <v>80</v>
+        <v>112</v>
       </c>
       <c r="D62" t="s">
         <v>9</v>
@@ -1829,13 +2005,13 @@
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="B63" t="s">
-        <v>82</v>
+        <v>114</v>
       </c>
       <c r="C63" t="s">
-        <v>83</v>
+        <v>115</v>
       </c>
       <c r="D63" t="s">
         <v>9</v>
@@ -1849,13 +2025,13 @@
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B64" t="s">
-        <v>7</v>
+        <v>105</v>
       </c>
       <c r="C64" t="s">
-        <v>80</v>
+        <v>106</v>
       </c>
       <c r="D64" t="s">
         <v>9</v>
@@ -1869,13 +2045,13 @@
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="B65" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="C65" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="D65" t="s">
         <v>9</v>
@@ -1889,13 +2065,13 @@
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="B66" t="s">
-        <v>7</v>
+        <v>121</v>
       </c>
       <c r="C66" t="s">
-        <v>80</v>
+        <v>122</v>
       </c>
       <c r="D66" t="s">
         <v>9</v>
@@ -1909,13 +2085,13 @@
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="B67" t="s">
-        <v>75</v>
+        <v>124</v>
       </c>
       <c r="C67" t="s">
-        <v>76</v>
+        <v>125</v>
       </c>
       <c r="D67" t="s">
         <v>9</v>
@@ -1929,13 +2105,13 @@
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>106</v>
+        <v>126</v>
       </c>
       <c r="B68" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="C68" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="D68" t="s">
         <v>9</v>
@@ -1949,13 +2125,13 @@
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>109</v>
+        <v>127</v>
       </c>
       <c r="B69" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="C69" t="s">
-        <v>111</v>
+        <v>129</v>
       </c>
       <c r="D69" t="s">
         <v>9</v>
@@ -1969,19 +2145,19 @@
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>112</v>
+        <v>130</v>
       </c>
       <c r="B70" t="s">
-        <v>103</v>
+        <v>131</v>
       </c>
       <c r="C70" t="s">
-        <v>102</v>
+        <v>132</v>
       </c>
       <c r="D70" t="s">
         <v>9</v>
       </c>
-      <c r="E70" t="s">
-        <v>51</v>
+      <c r="E70" t="s" s="1">
+        <v>10</v>
       </c>
       <c r="F70" t="s">
         <v>11</v>
@@ -1989,13 +2165,13 @@
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
       <c r="B71" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="C71" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="D71" t="s">
         <v>9</v>
@@ -2009,13 +2185,13 @@
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>114</v>
+        <v>134</v>
       </c>
       <c r="B72" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
       <c r="C72" t="s">
-        <v>116</v>
+        <v>136</v>
       </c>
       <c r="D72" t="s">
         <v>9</v>
@@ -2029,19 +2205,19 @@
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>117</v>
+        <v>137</v>
       </c>
       <c r="B73" t="s">
-        <v>107</v>
+        <v>7</v>
       </c>
       <c r="C73" t="s">
-        <v>108</v>
+        <v>138</v>
       </c>
       <c r="D73" t="s">
         <v>9</v>
       </c>
-      <c r="E73" t="s" s="1">
-        <v>10</v>
+      <c r="E73" t="s">
+        <v>51</v>
       </c>
       <c r="F73" t="s">
         <v>11</v>
@@ -2049,13 +2225,13 @@
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>118</v>
+        <v>139</v>
       </c>
       <c r="B74" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="C74" t="s">
-        <v>102</v>
+        <v>140</v>
       </c>
       <c r="D74" t="s">
         <v>9</v>
@@ -2069,13 +2245,13 @@
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>119</v>
+        <v>141</v>
       </c>
       <c r="B75" t="s">
-        <v>76</v>
+        <v>7</v>
       </c>
       <c r="C75" t="s">
-        <v>75</v>
+        <v>8</v>
       </c>
       <c r="D75" t="s">
         <v>9</v>
@@ -2089,13 +2265,13 @@
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>120</v>
+        <v>142</v>
       </c>
       <c r="B76" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C76" t="s">
-        <v>82</v>
+        <v>8</v>
       </c>
       <c r="D76" t="s">
         <v>9</v>
@@ -2109,19 +2285,19 @@
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>121</v>
+        <v>143</v>
       </c>
       <c r="B77" t="s">
-        <v>83</v>
+        <v>7</v>
       </c>
       <c r="C77" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D77" t="s">
         <v>9</v>
       </c>
-      <c r="E77" t="s">
-        <v>51</v>
+      <c r="E77" t="s" s="1">
+        <v>10</v>
       </c>
       <c r="F77" t="s">
         <v>11</v>
@@ -2129,19 +2305,19 @@
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>122</v>
+        <v>144</v>
       </c>
       <c r="B78" t="s">
-        <v>123</v>
+        <v>7</v>
       </c>
       <c r="C78" t="s">
-        <v>124</v>
+        <v>86</v>
       </c>
       <c r="D78" t="s">
         <v>9</v>
       </c>
-      <c r="E78" t="s">
-        <v>51</v>
+      <c r="E78" t="s" s="1">
+        <v>10</v>
       </c>
       <c r="F78" t="s">
         <v>11</v>
@@ -2149,21 +2325,341 @@
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>125</v>
+        <v>145</v>
       </c>
       <c r="B79" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C79" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="D79" t="s">
         <v>9</v>
       </c>
-      <c r="E79" t="s">
+      <c r="E79" t="s" s="1">
+        <v>10</v>
+      </c>
+      <c r="F79" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>146</v>
+      </c>
+      <c r="B80" t="s">
+        <v>7</v>
+      </c>
+      <c r="C80" t="s">
+        <v>86</v>
+      </c>
+      <c r="D80" t="s">
+        <v>9</v>
+      </c>
+      <c r="E80" t="s" s="1">
+        <v>10</v>
+      </c>
+      <c r="F80" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>147</v>
+      </c>
+      <c r="B81" t="s">
+        <v>148</v>
+      </c>
+      <c r="C81" t="s">
+        <v>149</v>
+      </c>
+      <c r="D81" t="s">
+        <v>9</v>
+      </c>
+      <c r="E81" t="s" s="1">
+        <v>10</v>
+      </c>
+      <c r="F81" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>150</v>
+      </c>
+      <c r="B82" t="s">
+        <v>7</v>
+      </c>
+      <c r="C82" t="s">
+        <v>86</v>
+      </c>
+      <c r="D82" t="s">
+        <v>9</v>
+      </c>
+      <c r="E82" t="s" s="1">
+        <v>10</v>
+      </c>
+      <c r="F82" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>151</v>
+      </c>
+      <c r="B83" t="s">
+        <v>88</v>
+      </c>
+      <c r="C83" t="s">
+        <v>89</v>
+      </c>
+      <c r="D83" t="s">
+        <v>9</v>
+      </c>
+      <c r="E83" t="s" s="1">
+        <v>10</v>
+      </c>
+      <c r="F83" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>152</v>
+      </c>
+      <c r="B84" t="s">
+        <v>153</v>
+      </c>
+      <c r="C84" t="s">
+        <v>154</v>
+      </c>
+      <c r="D84" t="s">
+        <v>9</v>
+      </c>
+      <c r="E84" t="s" s="1">
+        <v>10</v>
+      </c>
+      <c r="F84" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>155</v>
+      </c>
+      <c r="B85" t="s">
+        <v>156</v>
+      </c>
+      <c r="C85" t="s">
+        <v>157</v>
+      </c>
+      <c r="D85" t="s">
+        <v>9</v>
+      </c>
+      <c r="E85" t="s" s="1">
+        <v>10</v>
+      </c>
+      <c r="F85" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>158</v>
+      </c>
+      <c r="B86" t="s">
+        <v>156</v>
+      </c>
+      <c r="C86" t="s">
+        <v>157</v>
+      </c>
+      <c r="D86" t="s">
+        <v>9</v>
+      </c>
+      <c r="E86" t="s" s="1">
+        <v>10</v>
+      </c>
+      <c r="F86" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
+        <v>159</v>
+      </c>
+      <c r="B87" t="s">
+        <v>160</v>
+      </c>
+      <c r="C87" t="s">
+        <v>161</v>
+      </c>
+      <c r="D87" t="s">
+        <v>9</v>
+      </c>
+      <c r="E87" t="s" s="1">
+        <v>10</v>
+      </c>
+      <c r="F87" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s">
+        <v>162</v>
+      </c>
+      <c r="B88" t="s">
+        <v>163</v>
+      </c>
+      <c r="C88" t="s">
+        <v>164</v>
+      </c>
+      <c r="D88" t="s">
+        <v>9</v>
+      </c>
+      <c r="E88" t="s" s="1">
+        <v>10</v>
+      </c>
+      <c r="F88" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s">
+        <v>165</v>
+      </c>
+      <c r="B89" t="s">
+        <v>156</v>
+      </c>
+      <c r="C89" t="s">
+        <v>157</v>
+      </c>
+      <c r="D89" t="s">
+        <v>9</v>
+      </c>
+      <c r="E89" t="s" s="1">
+        <v>10</v>
+      </c>
+      <c r="F89" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s">
+        <v>166</v>
+      </c>
+      <c r="B90" t="s">
+        <v>160</v>
+      </c>
+      <c r="C90" t="s">
+        <v>161</v>
+      </c>
+      <c r="D90" t="s">
+        <v>9</v>
+      </c>
+      <c r="E90" t="s" s="1">
+        <v>10</v>
+      </c>
+      <c r="F90" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s">
+        <v>167</v>
+      </c>
+      <c r="B91" t="s">
+        <v>153</v>
+      </c>
+      <c r="C91" t="s">
+        <v>154</v>
+      </c>
+      <c r="D91" t="s">
+        <v>9</v>
+      </c>
+      <c r="E91" t="s" s="1">
+        <v>10</v>
+      </c>
+      <c r="F91" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s">
+        <v>168</v>
+      </c>
+      <c r="B92" t="s">
+        <v>89</v>
+      </c>
+      <c r="C92" t="s">
+        <v>88</v>
+      </c>
+      <c r="D92" t="s">
+        <v>9</v>
+      </c>
+      <c r="E92" t="s" s="1">
+        <v>10</v>
+      </c>
+      <c r="F92" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s">
+        <v>169</v>
+      </c>
+      <c r="B93" t="s">
+        <v>89</v>
+      </c>
+      <c r="C93" t="s">
+        <v>88</v>
+      </c>
+      <c r="D93" t="s">
+        <v>9</v>
+      </c>
+      <c r="E93" t="s">
         <v>51</v>
       </c>
-      <c r="F79" t="s">
+      <c r="F93" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s">
+        <v>170</v>
+      </c>
+      <c r="B94" t="s">
+        <v>171</v>
+      </c>
+      <c r="C94" t="s">
+        <v>172</v>
+      </c>
+      <c r="D94" t="s">
+        <v>9</v>
+      </c>
+      <c r="E94" t="s">
+        <v>51</v>
+      </c>
+      <c r="F94" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="s">
+        <v>173</v>
+      </c>
+      <c r="B95" t="s">
+        <v>89</v>
+      </c>
+      <c r="C95" t="s">
+        <v>88</v>
+      </c>
+      <c r="D95" t="s">
+        <v>9</v>
+      </c>
+      <c r="E95" t="s">
+        <v>51</v>
+      </c>
+      <c r="F95" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>